<commit_message>
Finishing Foundation Project Documentation
</commit_message>
<xml_diff>
--- a/Foundation Project Documents/Foundation Project Test Documentation.xlsx
+++ b/Foundation Project Documents/Foundation Project Test Documentation.xlsx
@@ -62,9 +62,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="120">
-  <si>
-    <t>ID: 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="130">
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>ID: 2</t>
@@ -156,6 +156,9 @@
     <t>Planets and Moons should allow adding an associated image, but an image should not be required for the data to be added to the database</t>
   </si>
   <si>
+    <t>User Stories</t>
+  </si>
+  <si>
     <t>given the user is on the login page</t>
   </si>
   <si>
@@ -283,6 +286,30 @@
   </si>
   <si>
     <t>and the user should remain on the home page without it updating</t>
+  </si>
+  <si>
+    <t>As a User I want to register a new account so I can track my discoveries in the Planetarium</t>
+  </si>
+  <si>
+    <t>As a User I want to log in to my account so I can manage my celestial discoveries</t>
+  </si>
+  <si>
+    <t>As a User I want to view the planets and moons in the Planetarium so I can learn about celestial bodies and new discoveries</t>
+  </si>
+  <si>
+    <t>As a User I want to add planets to the Planetarium so I can track and share my planetary data and findings</t>
+  </si>
+  <si>
+    <t>As a User I want to remove my Planets from the Planetarium so I can stop sharing my planetary discoveries</t>
+  </si>
+  <si>
+    <t>As a User I want to add moons to the Planetarium so I can display the relationships they have with planets</t>
+  </si>
+  <si>
+    <t>As a User I want to delete my moons from the Planetarium so I can remove the connection it has with a planet and its data</t>
+  </si>
+  <si>
+    <t>ID: 1</t>
   </si>
   <si>
     <t>Boundary Analysis Testing for 
@@ -293,7 +320,7 @@
 Planet name length</t>
   </si>
   <si>
-    <t>Boundary Analysis testing for the 
+    <t>Equivalence Partion testing for the 
 unique planet name entered for deletion</t>
   </si>
   <si>
@@ -301,7 +328,7 @@
 Moon name length</t>
   </si>
   <si>
-    <t>Boundary Analysis testing for the 
+    <t>Equivalence Partion testing for the 
 unique moon name entered for deletion</t>
   </si>
   <si>
@@ -331,13 +358,13 @@
     <t>Error Guess Testing to see if when a new planet is added, it is assigned to the respecitve user</t>
   </si>
   <si>
-    <t>Exploratory Testing to see if the user account Id matches the Owner Id of the planet within the source code</t>
+    <t>Exploratory Testing to see if the user account Id matches the Owner Id of the planet within the database</t>
   </si>
   <si>
     <t>Error Guess Testing to see if when a new Moon is added, it is assigned to the respective user and connected to a Planet</t>
   </si>
   <si>
-    <t>Exploratory Testing to see if the user account Id matches the Owner Id of the moon and there is a specified planet Id within the source code</t>
+    <t>Exploratory Testing to see if the user account Id matches the Owner Id of the moon and there is a specified planet Id within the database</t>
   </si>
   <si>
     <t>Error Guess Testing to see if the 
@@ -355,6 +382,9 @@
     <t>Error Guess Testing to see if a user who is the Owner of a planet can remove it and a user who is not the Owner cannot remove it</t>
   </si>
   <si>
+    <t>Error Guess Testing to see if moons can be successfully added to the Planetarium with or without an associated image</t>
+  </si>
+  <si>
     <t>Error Guess Testing to see if a user who is the Owner of a moon can remove it and a user who is not the Owner cannot remove it</t>
   </si>
   <si>
@@ -425,10 +455,10 @@
     <t>October 30th</t>
   </si>
   <si>
+    <t>October 31st</t>
+  </si>
+  <si>
     <t>6. Test Cycle Closure</t>
-  </si>
-  <si>
-    <t>October 31st</t>
   </si>
   <si>
     <t>Requirements Provided By Stakeholder</t>
@@ -448,7 +478,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="17">
+  <fonts count="14">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -483,25 +513,14 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="11.0"/>
-      <color rgb="FFE97132"/>
-      <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Aptos Narrow"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -516,7 +535,7 @@
     <font>
       <b/>
       <sz val="11.0"/>
-      <color theme="4"/>
+      <color rgb="FF156082"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -528,17 +547,12 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,14 +585,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF156082"/>
-        <bgColor rgb="FF156082"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4EA72E"/>
-        <bgColor rgb="FF4EA72E"/>
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
       </patternFill>
     </fill>
     <fill>
@@ -589,8 +597,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor theme="9"/>
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -643,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -668,60 +676,55 @@
     <xf borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="3" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="3" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="9" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="9" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="8" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="8" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="11" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="8" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="11" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1018,7 +1021,7 @@
       <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1033,7 +1036,7 @@
       <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1073,13 +1076,13 @@
       <c r="E5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1095,223 +1098,249 @@
         <v>28</v>
       </c>
       <c r="G6" s="7"/>
+      <c r="J6" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>31</v>
+      <c r="D7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="9" t="s">
         <v>38</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="F9" s="9" t="s">
         <v>45</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="13" t="s">
         <v>47</v>
       </c>
+      <c r="B10" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="C10" s="12"/>
-      <c r="D10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="E10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>51</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>53</v>
+      <c r="D11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>31</v>
+      <c r="A12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="15" t="s">
+      <c r="C13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="E13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="G13" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="D14" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="G14" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="E15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="F15" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="G15" s="10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15" t="s">
+      <c r="A16" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>71</v>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2316,179 +2345,179 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>74</v>
+        <v>82</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>82</v>
+        <v>90</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>84</v>
+        <v>92</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>86</v>
+        <v>94</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>88</v>
+        <v>96</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>89</v>
+        <v>99</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>93</v>
+      <c r="A7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>95</v>
+      <c r="A8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2523,80 +2552,96 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>99</v>
+      <c r="A1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22" t="s">
-        <v>102</v>
+      <c r="A2" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="20" t="s">
-        <v>105</v>
+      <c r="A3" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25" t="s">
-        <v>108</v>
+      <c r="A4" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>111</v>
+      <c r="A5" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>113</v>
-      </c>
+      <c r="A6" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="23"/>
     </row>
     <row r="7">
-      <c r="A7" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>115</v>
+      <c r="A7" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2638,23 +2683,23 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
-        <v>116</v>
+      <c r="A1" s="18" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="27" t="s">
-        <v>117</v>
+      <c r="A2" s="24" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="27" t="s">
-        <v>118</v>
+      <c r="A3" s="24" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="27" t="s">
-        <v>119</v>
+      <c r="A4" s="24" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>